<commit_message>
use nrces fhir profiles for common resources
</commit_message>
<xml_diff>
--- a/v0.7/StructureDefinition-CoverageEligibilityRequest.xlsx
+++ b/v0.7/StructureDefinition-CoverageEligibilityRequest.xlsx
@@ -544,7 +544,7 @@
     <t>CoverageEligibilityRequest.patient</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(Patient)
+    <t xml:space="preserve">Reference(https://nrces.in/ndhm/fhir/r4/StructureDefinition/Patient)
 </t>
   </si>
   <si>
@@ -610,7 +610,7 @@
     <t>CoverageEligibilityRequest.enterer</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(Practitioner|PractitionerRole)
+    <t xml:space="preserve">Reference(https://nrces.in/ndhm/fhir/r4/StructureDefinition/Practitioner|https://nrces.in/ndhm/fhir/r4/StructureDefinition/PractitionerRole)
 </t>
   </si>
   <si>
@@ -629,7 +629,7 @@
     <t>CoverageEligibilityRequest.provider</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(Practitioner|Organization)
+    <t xml:space="preserve">Reference(https://nrces.in/ndhm/fhir/r4/StructureDefinition/Practitioner|https://nrces.in/ndhm/fhir/r4/StructureDefinition/Organization)
 </t>
   </si>
   <si>
@@ -654,7 +654,7 @@
     <t>CoverageEligibilityRequest.insurer</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(Organization)
+    <t xml:space="preserve">Reference(https://nrces.in/ndhm/fhir/r4/StructureDefinition/Organization)
 </t>
   </si>
   <si>
@@ -845,7 +845,7 @@
     <t>CoverageEligibilityRequest.insurance.coverage</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(Coverage)
+    <t xml:space="preserve">Reference(https://swasth-digital-health-foundation.github.io/standards/v0.7/StructureDefinition-Coverage.html)
 </t>
   </si>
   <si>
@@ -1010,7 +1010,7 @@
     <t>CoverageEligibilityRequest.item.facility</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(Location|Organization)
+    <t xml:space="preserve">Reference(Location|https://nrces.in/ndhm/fhir/r4/StructureDefinition/Organization)
 </t>
   </si>
   <si>
@@ -1042,7 +1042,7 @@
   </si>
   <si>
     <t>CodeableConcept
-Reference(Condition)</t>
+Reference(https://nrces.in/ndhm/fhir/r4/StructureDefinition/Condition)</t>
   </si>
   <si>
     <t>Nature of illness or problem</t>

</xml_diff>